<commit_message>
Added Sheet3 for Output
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vybha\Desktop\Hackathon2024\Hackathon2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4DC3ED5-165D-4EEF-82F8-064ECB094824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBFEF31-045D-447B-BFAC-685C0C824332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22620" yWindow="1035" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{BC51CB07-A3CD-46D9-8A0D-2CC36C58E82C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{BC51CB07-A3CD-46D9-8A0D-2CC36C58E82C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Aconnect</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -103,9 +109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -442,18 +452,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00ADEF69-50E3-4A58-A6A4-1486D80C3664}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A12" sqref="A12:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -471,7 +485,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -480,6 +494,20 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -490,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB7AB18-ABB8-4E50-977D-4E3205BBBF8D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,4 +555,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A15388-6148-4B79-9109-12D66D9876A4}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="33.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>